<commit_message>
Se actualizaron las tareas realizadas y se agregaron las tareas que falta terminar cuanto antes, para poder continuar con la siguiente etapa.
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>TAREAS</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Trabajando</t>
-  </si>
-  <si>
-    <t>Agregar comportamientos jquery</t>
   </si>
   <si>
     <t>Incompleto</t>
@@ -74,15 +71,6 @@
     <t>Falta crear la parte de compra.</t>
   </si>
   <si>
-    <t>Se crearon los scripts para:
-Index: Slider de productos destacados.
-Tienda: Visualización de imágenes.
-Contacto: Validación de Formulario.
-Producto: Validación de un valor de productos.
-*: Igualación en la altura de las comlumnas.
-(Cada página, tiene su propio archivo .js dentro de la carpeta js/secciones).</t>
-  </si>
-  <si>
     <t>Combinación de para parte estática con la dinámica</t>
   </si>
   <si>
@@ -97,7 +85,77 @@
      * Cambiar el escrip de la visualización de detalle. En vez de que sea por terminación de punto, que sea por cantidad de palabras.</t>
   </si>
   <si>
-    <t>Vinculación de los productos con Redes Sociales (Facebook y Twitter)</t>
+    <t>Agregar Jquery Slider - INDEX</t>
+  </si>
+  <si>
+    <t>Index: Slider de productos destacados y más vendidos.</t>
+  </si>
+  <si>
+    <t>Agregar Jquery imagenes - TIENDA</t>
+  </si>
+  <si>
+    <t>Tienda: Visualización de imágenes.</t>
+  </si>
+  <si>
+    <t>Agregar Jquery validación formularios - CONTACTO/PRODUCTO</t>
+  </si>
+  <si>
+    <t>*: Igualación en la altura de las comlumnas para todas las seccions.</t>
+  </si>
+  <si>
+    <t>Contacto: Validación de Formulario.
+Producto: Validación de un valor de productos.</t>
+  </si>
+  <si>
+    <t>Agregar Jquery altura de columnas - TODAS LAS SECCIONES</t>
+  </si>
+  <si>
+    <t>Agregar comportamientos para redes sociales</t>
+  </si>
+  <si>
+    <t>Ya esta completo para Twitter y Facebook, falta el RSS</t>
+  </si>
+  <si>
+    <t>Finalizar Index</t>
+  </si>
+  <si>
+    <t>Queda refinar los estilos de los sliders y agregar información</t>
+  </si>
+  <si>
+    <t>Cambiar el texto formulario - CONTACTO</t>
+  </si>
+  <si>
+    <t>Debo pedir el texto al cliente para cambiarlo</t>
+  </si>
+  <si>
+    <t>Resolver símbolos raros en los textos y títulos</t>
+  </si>
+  <si>
+    <t>Salen símbolos raros para la letra Ñ y aquellas letras con acento</t>
+  </si>
+  <si>
+    <t>Cambiar imágenes al visualizar los productos</t>
+  </si>
+  <si>
+    <t>Se debe mostrar la imagen del producto seleccionado. Actualmente se muestra siempre la misma imagen para todos los productos</t>
+  </si>
+  <si>
+    <t>Falta crear las imágenes y likearlas a la url respectiva</t>
+  </si>
+  <si>
+    <t>ESTAMOS TODO EL TIEMPO ACTUALIZANDO</t>
+  </si>
+  <si>
+    <t>Cambiar las imágenes de los banners - Lateral Derecho</t>
+  </si>
+  <si>
+    <t>Agregar imágenes redes sociales - Lateral Derecho</t>
+  </si>
+  <si>
+    <t>Crear script para banner superior - INDEX</t>
+  </si>
+  <si>
+    <t>Debo pedir las imágenes fuentes</t>
   </si>
 </sst>
 </file>
@@ -190,12 +248,75 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -207,37 +328,61 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -541,149 +686,294 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="63.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="19.5" thickBot="1">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30">
+      <c r="A9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="75">
+      <c r="A17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45">
+      <c r="A18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="135">
-      <c r="A7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="B20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="90">
-      <c r="A8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>12</v>
+      <c r="D20" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ahora toma bien la imagen en el prod_info
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -11,7 +11,7 @@
     <sheet name="Issues" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -77,14 +77,6 @@
     <t>Fanky, Marcelo</t>
   </si>
   <si>
-    <t>Visaulización productos, sección TIENDA</t>
-  </si>
-  <si>
-    <t>Falta:
-     * El poder seleccionar la forma en que se visualizan los productos en la tienda.
-     * Cambiar el escrip de la visualización de detalle. En vez de que sea por terminación de punto, que sea por cantidad de palabras.</t>
-  </si>
-  <si>
     <t>Agregar Jquery Slider - INDEX</t>
   </si>
   <si>
@@ -156,6 +148,14 @@
   </si>
   <si>
     <t>Debo pedir las imágenes fuentes</t>
+  </si>
+  <si>
+    <t>Visualización productos, sección TIENDA</t>
+  </si>
+  <si>
+    <t>Falta:
+     * El poder seleccionar la forma en que se visualizan los productos en la tienda. (ese combo box limeta)
+     * Cambiar el script de la visualización de detalle. En vez de que sea por terminación de punto, que sea por cantidad de palabras.</t>
   </si>
 </sst>
 </file>
@@ -328,7 +328,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -345,9 +345,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -357,9 +354,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -383,6 +377,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -688,8 +691,8 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -701,21 +704,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -724,12 +727,12 @@
       <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -738,12 +741,12 @@
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -752,65 +755,67 @@
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>16</v>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" ht="75">
+      <c r="A5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45">
+      <c r="A6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>22</v>
+      <c r="A7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30">
-      <c r="A9" s="8" t="s">
-        <v>25</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
@@ -818,97 +823,95 @@
       <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>27</v>
-      </c>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="A10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>30</v>
+      <c r="D11" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>32</v>
+        <v>23</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>39</v>
+        <v>26</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>39</v>
+      <c r="A15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="7" t="s">
-        <v>43</v>
+      <c r="A16" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>8</v>
@@ -916,67 +919,70 @@
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="75">
-      <c r="A17" s="7" t="s">
-        <v>19</v>
+      <c r="D16" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="45">
-      <c r="A18" s="7" t="s">
-        <v>37</v>
+      <c r="D17" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>38</v>
+      <c r="D18" s="11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="7" t="s">
-        <v>35</v>
+      <c r="A19" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="13" t="s">
-        <v>36</v>
+      <c r="D19" s="11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>40</v>
+      <c r="A20" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:D20">
+    <sortCondition ref="B3"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
actualice las tareas a realizar y modifique una pavada del input de la cantidad de productos.
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -11,12 +11,12 @@
     <sheet name="Issues" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
   <si>
     <t>TAREAS</t>
   </si>
@@ -68,15 +68,6 @@
     <t>Falta agregar las imágenes a la BD.</t>
   </si>
   <si>
-    <t>Falta crear la parte de compra.</t>
-  </si>
-  <si>
-    <t>Combinación de para parte estática con la dinámica</t>
-  </si>
-  <si>
-    <t>Fanky, Marcelo</t>
-  </si>
-  <si>
     <t>Agregar Jquery Slider - INDEX</t>
   </si>
   <si>
@@ -105,9 +96,6 @@
     <t>Agregar comportamientos para redes sociales</t>
   </si>
   <si>
-    <t>Ya esta completo para Twitter y Facebook, falta el RSS</t>
-  </si>
-  <si>
     <t>Finalizar Index</t>
   </si>
   <si>
@@ -130,12 +118,6 @@
   </si>
   <si>
     <t>Se debe mostrar la imagen del producto seleccionado. Actualmente se muestra siempre la misma imagen para todos los productos</t>
-  </si>
-  <si>
-    <t>Falta crear las imágenes y likearlas a la url respectiva</t>
-  </si>
-  <si>
-    <t>ESTAMOS TODO EL TIEMPO ACTUALIZANDO</t>
   </si>
   <si>
     <t>Cambiar las imágenes de los banners - Lateral Derecho</t>
@@ -156,13 +138,22 @@
     <t>Falta:
      * El poder seleccionar la forma en que se visualizan los productos en la tienda. (ese combo box limeta)
      * Cambiar el script de la visualización de detalle. En vez de que sea por terminación de punto, que sea por cantidad de palabras.</t>
+  </si>
+  <si>
+    <t>Esta completa en las seccions cart, checkout01 y 02, falta la FACTURA</t>
+  </si>
+  <si>
+    <t>Se completo, con los banners laterales incluido.</t>
+  </si>
+  <si>
+    <t>Ya esta completo para Twitter y Facebook, falta el el envio a un mail.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,13 +164,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,11 +209,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -320,80 +299,72 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
-    <cellStyle name="Énfasis1" xfId="4" builtinId="29"/>
-    <cellStyle name="Énfasis2" xfId="5" builtinId="33"/>
-    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Énfasis1" xfId="3" builtinId="29"/>
+    <cellStyle name="Énfasis2" xfId="4" builtinId="33"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -689,10 +660,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -700,7 +671,7 @@
     <col min="1" max="1" width="57.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" thickBot="1">
@@ -759,7 +730,7 @@
     </row>
     <row r="5" spans="1:4" ht="75">
       <c r="A5" s="6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>4</v>
@@ -768,12 +739,12 @@
         <v>11</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45">
       <c r="A6" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
@@ -782,12 +753,12 @@
         <v>11</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
@@ -796,52 +767,54 @@
         <v>11</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>8</v>
@@ -850,12 +823,12 @@
         <v>5</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30">
+      <c r="A12" s="7" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>8</v>
@@ -863,11 +836,11 @@
       <c r="C12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
@@ -877,41 +850,41 @@
       <c r="C13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="D13" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30">
+      <c r="A14" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="B14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="10" t="s">
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>8</v>
@@ -920,63 +893,45 @@
         <v>11</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="A17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>42</v>
+      <c r="D19" s="17" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lista de productos con ordenamiento (basico) mas ajax (anda por ahora.. jeje)
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -11,7 +11,7 @@
     <sheet name="Issues" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -662,8 +662,8 @@
   </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -742,17 +742,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:4" ht="30">
+      <c r="A6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="11" t="s">
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
mejorar la lista de productos, se puede hacer llamando la funcion a una lib de js.. charlar con marcelo tareas upd solo me falta lo de los simbolos x)
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -662,8 +662,8 @@
   </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -729,16 +729,16 @@
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" ht="75">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
actualice las tareas y limpie un poco el codigo para que e. jquery esté en su respectivo archivo.
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -11,12 +11,12 @@
     <sheet name="Issues" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>TAREAS</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Cambiar imágenes al visualizar los productos</t>
   </si>
   <si>
-    <t>Se debe mostrar la imagen del producto seleccionado. Actualmente se muestra siempre la misma imagen para todos los productos</t>
-  </si>
-  <si>
     <t>Cambiar las imágenes de los banners - Lateral Derecho</t>
   </si>
   <si>
@@ -133,11 +130,6 @@
   </si>
   <si>
     <t>Visualización productos, sección TIENDA</t>
-  </si>
-  <si>
-    <t>Falta:
-     * El poder seleccionar la forma en que se visualizan los productos en la tienda. (ese combo box limeta)
-     * Cambiar el script de la visualización de detalle. En vez de que sea por terminación de punto, que sea por cantidad de palabras.</t>
   </si>
   <si>
     <t>Esta completa en las seccions cart, checkout01 y 02, falta la FACTURA</t>
@@ -662,8 +654,8 @@
   </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -728,9 +720,9 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" ht="75">
+    <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
@@ -738,11 +730,9 @@
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30">
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
         <v>31</v>
       </c>
@@ -752,9 +742,7 @@
       <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
@@ -781,7 +769,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -795,7 +783,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -854,7 +842,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30">
+    <row r="14" spans="1:4" ht="19.5" customHeight="1">
       <c r="A14" s="8" t="s">
         <v>24</v>
       </c>
@@ -865,7 +853,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -898,7 +886,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>8</v>
@@ -910,7 +898,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>8</v>
@@ -922,7 +910,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>8</v>
@@ -931,7 +919,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se actualizaron las tareas. Se agregó el banner superior, junto con todas las imagenes y textos pertinentes. Además el mismo ha sido animado con el jquery.
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
   <si>
     <t>TAREAS</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Crear script para banner superior - INDEX</t>
   </si>
   <si>
-    <t>Debo pedir las imágenes fuentes</t>
-  </si>
-  <si>
     <t>Visualización productos, sección TIENDA</t>
   </si>
   <si>
@@ -139,6 +136,12 @@
   </si>
   <si>
     <t>Ya esta completo para Twitter y Facebook, falta el el envio a un mail.</t>
+  </si>
+  <si>
+    <t>Completar el proceso de compra</t>
+  </si>
+  <si>
+    <t>Tiene que poder agregarse productos al carrito y luego realizar los pasos necesario para la compra. Al finalizar mostrar una factura, al mismo tiempo que sea emitida al cliente y al administrador.</t>
   </si>
 </sst>
 </file>
@@ -342,13 +345,13 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -652,10 +655,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -722,7 +725,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
@@ -744,9 +747,9 @@
       </c>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="45">
       <c r="A7" s="6" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
@@ -755,124 +758,124 @@
         <v>11</v>
       </c>
       <c r="D7" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="7" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="8" t="s">
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>17</v>
+      <c r="D10" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="B12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30">
-      <c r="A12" s="7" t="s">
+    <row r="13" spans="1:4" ht="30">
+      <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="B13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="7" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="19.5" customHeight="1">
-      <c r="A14" s="8" t="s">
+    <row r="15" spans="1:4" ht="19.5" customHeight="1">
+      <c r="A15" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="B15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>28</v>
+      <c r="D15" s="10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>8</v>
@@ -881,46 +884,58 @@
         <v>11</v>
       </c>
       <c r="D16" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="9"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="15" t="s">
+      <c r="B19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>35</v>
-      </c>
+      <c r="B20" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="17"/>
     </row>
   </sheetData>
   <sortState ref="A2:D20">

</xml_diff>

<commit_message>
agregado de la columna de cant horas (que se piensa hacer o se ha logrado el objetivo)
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -11,12 +11,12 @@
     <sheet name="Issues" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
   <si>
     <t>TAREAS</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>Queda finalizar los banner debajo del slider para acceso directo a las secciones.</t>
+  </si>
+  <si>
+    <t>Cant Horas</t>
+  </si>
+  <si>
+    <t>Listado de Productos con ordenamiento</t>
+  </si>
+  <si>
+    <t>Uso minimo de jquey + AJAX</t>
   </si>
 </sst>
 </file>
@@ -225,7 +234,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -294,6 +303,26 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -304,7 +333,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -356,6 +385,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -658,10 +696,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -670,9 +708,10 @@
     <col min="2" max="2" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" thickBot="1">
+    <row r="1" spans="1:5" ht="19.5" thickBot="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -685,8 +724,11 @@
       <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="45">
+      <c r="E1" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -699,36 +741,44 @@
       <c r="D2" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="6" t="s">
+      <c r="E2" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="7" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
@@ -736,11 +786,14 @@
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" s="7"/>
+      <c r="E5" s="20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>4</v>
@@ -749,24 +802,24 @@
         <v>5</v>
       </c>
       <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="45">
-      <c r="A7" s="6" t="s">
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:5" ht="45">
+      <c r="A8" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
@@ -775,12 +828,12 @@
         <v>11</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
@@ -789,122 +842,122 @@
         <v>11</v>
       </c>
       <c r="D9" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="7" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="7" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="7" t="s">
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="B13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="7" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30">
-      <c r="A14" s="7" t="s">
+    <row r="15" spans="1:5" ht="30">
+      <c r="A15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="9" t="s">
+      <c r="B15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="7" t="s">
+    <row r="16" spans="1:5">
+      <c r="A16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="B16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="19.5" customHeight="1">
-      <c r="A16" s="8" t="s">
+    <row r="17" spans="1:4" ht="19.5" customHeight="1">
+      <c r="A17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="B17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="6" t="s">
+    <row r="18" spans="1:4">
+      <c r="A18" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30">
-      <c r="A18" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>8</v>
@@ -913,49 +966,66 @@
         <v>11</v>
       </c>
       <c r="D18" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30">
+      <c r="A19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="15" t="s">
+      <c r="B21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="17"/>
+      <c r="B22" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="17"/>
     </row>
   </sheetData>
   <sortState ref="A2:D20">
     <sortCondition ref="B3"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="E5:E7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
nuevas tareas y un poco de logica en el checkout02.php para preguntar e implementar
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -11,12 +11,12 @@
     <sheet name="Issues" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
   <si>
     <t>TAREAS</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Carga completa de los datos (incluyendo imágenes)</t>
   </si>
   <si>
-    <t>Falta agregar las imágenes a la BD.</t>
-  </si>
-  <si>
     <t>Agregar Jquery Slider - INDEX</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>Listado de Productos con ordenamiento</t>
   </si>
   <si>
-    <t>Uso minimo de jquey + AJAX</t>
-  </si>
-  <si>
     <t>Pusimos categorías que nos parecieron a nosotros, si el cliente quiere cambiarlas que abone los banners.</t>
   </si>
   <si>
@@ -168,6 +162,15 @@
   </si>
   <si>
     <t>Separa los archivos de acuerdo su utilizacion y posicion para la web.</t>
+  </si>
+  <si>
+    <t>Cargadas todas las imagenes correctamentes (+ enlace con el producto)</t>
+  </si>
+  <si>
+    <t>Uso minimo de jquery + AJAX</t>
+  </si>
+  <si>
+    <t>Al cargar con ajax la segunda pagina del listado de productos se rompe el listado de categorias</t>
   </si>
 </sst>
 </file>
@@ -326,7 +329,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -370,9 +373,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -397,6 +397,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -701,18 +707,18 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="18"/>
+    <col min="1" max="1" width="57.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" customFormat="1" ht="19.5" thickBot="1">
@@ -729,7 +735,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" customFormat="1" ht="45">
@@ -751,7 +757,7 @@
     </row>
     <row r="3" spans="1:5" customFormat="1">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -760,24 +766,24 @@
         <v>5</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E3" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" customFormat="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>15</v>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5" customFormat="1">
@@ -791,13 +797,13 @@
         <v>5</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="15">
+      <c r="E5" s="24">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -806,11 +812,11 @@
         <v>5</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="15"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -819,11 +825,11 @@
         <v>5</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="15"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:5" customFormat="1" ht="45">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -832,12 +838,12 @@
         <v>11</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1">
       <c r="A9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
@@ -846,12 +852,12 @@
         <v>11</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
@@ -860,7 +866,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" customFormat="1">
@@ -874,7 +880,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1">
@@ -891,35 +897,35 @@
     </row>
     <row r="13" spans="1:5" customFormat="1">
       <c r="A13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" customFormat="1">
       <c r="A14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5" customFormat="1" ht="30">
       <c r="A15" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
@@ -928,12 +934,12 @@
         <v>5</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1">
       <c r="A16" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
@@ -942,12 +948,12 @@
         <v>5</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" customFormat="1" ht="19.5" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>8</v>
@@ -956,12 +962,12 @@
         <v>10</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" customFormat="1">
       <c r="A18" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
@@ -970,12 +976,12 @@
         <v>11</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" customFormat="1" ht="30">
       <c r="A19" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>8</v>
@@ -984,37 +990,37 @@
         <v>5</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" customFormat="1">
       <c r="A20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" customFormat="1">
+      <c r="A21" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" customFormat="1">
+      <c r="A22" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="1:4" customFormat="1">
-      <c r="A21" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:4" customFormat="1">
-      <c r="A22" s="16" t="s">
-        <v>33</v>
-      </c>
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1024,8 +1030,8 @@
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" customFormat="1" ht="30">
-      <c r="A23" s="19" t="s">
-        <v>45</v>
+      <c r="A23" s="18" t="s">
+        <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
@@ -1034,12 +1040,12 @@
         <v>11</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="20" t="s">
-        <v>47</v>
+      <c r="A24" s="19" t="s">
+        <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1048,43 +1054,46 @@
         <v>11</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="22"/>
+      <c r="A25" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="21"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="21"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="21"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="21"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="22"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="21"/>
     </row>
   </sheetData>
   <sortState ref="A2:D20">

</xml_diff>

<commit_message>
actualizacion de tareas y checkout.php que destruye la session y envia email (falta por falta de conocimiento)
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -132,9 +132,6 @@
     <t>Completar el proceso de compra</t>
   </si>
   <si>
-    <t>Tiene que poder agregarse productos al carrito y luego realizar los pasos necesario para la compra. Al finalizar mostrar una factura, al mismo tiempo que sea emitida al cliente y al administrador.</t>
-  </si>
-  <si>
     <t>Buscador</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>Al cargar con ajax la segunda pagina del listado de productos se rompe el listado de categorias</t>
+  </si>
+  <si>
+    <t>Al finalizar mostrar una factura, al mismo tiempo que sea emitida al cliente y al administrador. Ayuda con este tema!</t>
   </si>
 </sst>
 </file>
@@ -398,11 +398,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -707,8 +707,8 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -735,7 +735,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" customFormat="1" ht="45">
@@ -757,7 +757,7 @@
     </row>
     <row r="3" spans="1:5" customFormat="1">
       <c r="A3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -766,7 +766,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="14">
         <v>6</v>
@@ -783,7 +783,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" customFormat="1">
@@ -797,7 +797,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="24">
+      <c r="E5" s="25">
         <v>12</v>
       </c>
     </row>
@@ -812,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="24"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:5" customFormat="1">
       <c r="A7" s="5" t="s">
@@ -825,9 +825,9 @@
         <v>5</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="24"/>
-    </row>
-    <row r="8" spans="1:5" customFormat="1" ht="45">
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" customFormat="1" ht="30">
       <c r="A8" s="4" t="s">
         <v>36</v>
       </c>
@@ -838,12 +838,12 @@
         <v>11</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1">
       <c r="A9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
@@ -852,7 +852,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1">
@@ -990,7 +990,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" customFormat="1">
@@ -1031,7 +1031,7 @@
     </row>
     <row r="23" spans="1:4" customFormat="1" ht="30">
       <c r="A23" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
@@ -1040,12 +1040,12 @@
         <v>11</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1054,12 +1054,12 @@
         <v>11</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="25" t="s">
-        <v>49</v>
+      <c r="A25" s="24" t="s">
+        <v>48</v>
       </c>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>

</xml_diff>

<commit_message>
modificacion nombre checkout.php a envio_checkout.php tareas modificadas producto_info ahora redirecciona correctamente
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -167,10 +167,11 @@
     <t>Uso minimo de jquery + AJAX</t>
   </si>
   <si>
-    <t>Al cargar con ajax la segunda pagina del listado de productos se rompe el listado de categorias</t>
-  </si>
-  <si>
     <t>Al finalizar mostrar una factura, al mismo tiempo que sea emitida al cliente y al administrador. Ayuda con este tema!</t>
+  </si>
+  <si>
+    <t>Al cargar con ajax la segunda pagina del listado de productos
+se rompe el listado de categorias</t>
   </si>
 </sst>
 </file>
@@ -395,13 +396,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -707,8 +708,8 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -838,7 +839,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1">
@@ -1030,7 +1031,7 @@
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" customFormat="1" ht="30">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="23" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1057,9 +1058,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="23" t="s">
-        <v>48</v>
+    <row r="25" spans="1:4" ht="30">
+      <c r="A25" s="25" t="s">
+        <v>49</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>

</xml_diff>

<commit_message>
modificacion de la lista de tareas...
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="50">
   <si>
     <t>TAREAS</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Resolver símbolos raros en los textos y títulos</t>
   </si>
   <si>
-    <t>Salen símbolos raros para la letra Ñ y aquellas letras con acento</t>
-  </si>
-  <si>
     <t>Cambiar imágenes al visualizar los productos</t>
   </si>
   <si>
@@ -167,11 +164,14 @@
     <t>Uso minimo de jquery + AJAX</t>
   </si>
   <si>
-    <t>Al finalizar mostrar una factura, al mismo tiempo que sea emitida al cliente y al administrador. Ayuda con este tema!</t>
-  </si>
-  <si>
     <t>Al cargar con ajax la segunda pagina del listado de productos
 se rompe el listado de categorias</t>
+  </si>
+  <si>
+    <t>Al finalizar mostrar una factura, revisar si le llega al administrador</t>
+  </si>
+  <si>
+    <t>fixed ñ + vocales con tildes</t>
   </si>
 </sst>
 </file>
@@ -330,7 +330,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -401,9 +401,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -708,8 +705,8 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -736,7 +733,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" customFormat="1" ht="45">
@@ -758,7 +755,7 @@
     </row>
     <row r="3" spans="1:5" customFormat="1">
       <c r="A3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -767,7 +764,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="14">
         <v>6</v>
@@ -784,7 +781,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" customFormat="1">
@@ -804,7 +801,7 @@
     </row>
     <row r="6" spans="1:5" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -817,7 +814,7 @@
     </row>
     <row r="7" spans="1:5" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -828,23 +825,23 @@
       <c r="D7" s="7"/>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:5" customFormat="1" ht="30">
-      <c r="A8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="1:5" customFormat="1">
+      <c r="A8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1">
       <c r="A9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
@@ -853,21 +850,21 @@
         <v>11</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" customFormat="1">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>28</v>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" customFormat="1">
@@ -881,7 +878,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" customFormat="1">
@@ -963,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" customFormat="1">
@@ -991,12 +988,12 @@
         <v>5</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" customFormat="1">
       <c r="A20" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>8</v>
@@ -1008,7 +1005,7 @@
     </row>
     <row r="21" spans="1:4" customFormat="1">
       <c r="A21" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>8</v>
@@ -1020,7 +1017,7 @@
     </row>
     <row r="22" spans="1:4" customFormat="1">
       <c r="A22" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>8</v>
@@ -1032,7 +1029,7 @@
     </row>
     <row r="23" spans="1:4" customFormat="1" ht="30">
       <c r="A23" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>4</v>
@@ -1041,12 +1038,12 @@
         <v>5</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1055,16 +1052,20 @@
         <v>11</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30">
-      <c r="A25" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="20"/>
+      <c r="A25" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4">
       <c r="B26" s="21"/>

</xml_diff>

<commit_message>
arrgle todos los errores de .js que había, tanto en la home como la visualizacion de productos. Actualce las tareas.
ERROR: ahora no funca el ordenar, o sea, anda, pero no muestra.
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -11,12 +11,12 @@
     <sheet name="Issues" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
   <si>
     <t>TAREAS</t>
   </si>
@@ -172,13 +172,46 @@
   </si>
   <si>
     <t>fixed ñ + vocales con tildes</t>
+  </si>
+  <si>
+    <t>Arreglar Bugs</t>
+  </si>
+  <si>
+    <t>Index: slider no funciona.</t>
+  </si>
+  <si>
+    <t>Tienda: no funciona el agrandar imagenes</t>
+  </si>
+  <si>
+    <t>Producto: faltan modificar los estilos.</t>
+  </si>
+  <si>
+    <t>Falta agregar el mostrar que se cargo correctamente el producto.</t>
+  </si>
+  <si>
+    <t>Contacto: faltan estilos del boton de enviar.</t>
+  </si>
+  <si>
+    <t>Checkput: agregar estilos. ERROR AL ACTUALIZAR/BORRAR DATOS LAS CANTIDADES</t>
+  </si>
+  <si>
+    <t>Checkout1: agregar las validaciones</t>
+  </si>
+  <si>
+    <t>Factura, ponerla a dentro de el archivo factura.php</t>
+  </si>
+  <si>
+    <t>FALTA QUE LLEGUE AL ADMINISTRADOR TAMBIEN</t>
+  </si>
+  <si>
+    <t>Falta arreglar el ordenar en las tiendas.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,8 +248,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,8 +283,13 @@
         <fgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -322,15 +367,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -387,26 +455,39 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Énfasis1" xfId="3" builtinId="29"/>
     <cellStyle name="Énfasis2" xfId="4" builtinId="33"/>
+    <cellStyle name="Incorrecto" xfId="5" builtinId="27"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -703,18 +784,18 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="57.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="11.42578125" style="17"/>
   </cols>
@@ -1028,7 +1109,7 @@
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" customFormat="1" ht="30">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1056,7 +1137,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="30">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1068,34 +1149,90 @@
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="20"/>
+      <c r="A26" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="25"/>
+      <c r="D26" s="22" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="20"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="22" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="20"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="20"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="20"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="20"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="23"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="23"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="23"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="26"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="28" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:D20">

</xml_diff>

<commit_message>
mejore el funcionamiento y visualizacion del formulario de contacto.php. agregue y actualice las tareas.
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="66">
   <si>
     <t>TAREAS</t>
   </si>
@@ -148,10 +148,6 @@
  muestre correctamente</t>
   </si>
   <si>
-    <t>Agregar al js para mostrar/ocultar el carrito.
-Ver script para actulizar listado al borrar un producto.</t>
-  </si>
-  <si>
     <t>Acomodar los archivos en carpetas correctamente</t>
   </si>
   <si>
@@ -205,6 +201,26 @@
   </si>
   <si>
     <t>Falta arreglar el ordenar en las tiendas.</t>
+  </si>
+  <si>
+    <t>Fanky/Marcelo</t>
+  </si>
+  <si>
+    <t>Falta validar los campos antes de continuar</t>
+  </si>
+  <si>
+    <t>Falta cargar todas las zonas de envio</t>
+  </si>
+  <si>
+    <t>Select de checkout01.php</t>
+  </si>
+  <si>
+    <t>Validar entrada a la facturacion</t>
+  </si>
+  <si>
+    <t>Solo se prodra acceder a checkout01.php si primeramente en cart.php tiene artículos cargados.
+Solo se podrá acceder a checkout02.php si completó correctamente los datos de checkout01.php.
+Solo podrá acceder a factura.php y enviar correctamente el mail, si esta completo correctamente todo lo que existe en checkout02.php</t>
   </si>
 </sst>
 </file>
@@ -249,14 +265,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,11 +300,6 @@
         <fgColor theme="5"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -390,13 +402,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -461,33 +472,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Énfasis1" xfId="3" builtinId="29"/>
     <cellStyle name="Énfasis2" xfId="4" builtinId="33"/>
-    <cellStyle name="Incorrecto" xfId="5" builtinId="27"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -784,10 +794,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -845,7 +855,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="14">
         <v>6</v>
@@ -862,7 +872,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" customFormat="1">
@@ -876,7 +886,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <v>12</v>
       </c>
     </row>
@@ -891,7 +901,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="E6" s="24"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:5" customFormat="1">
       <c r="A7" s="5" t="s">
@@ -904,7 +914,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="24"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="1:5" customFormat="1">
       <c r="A8" s="6" t="s">
@@ -917,7 +927,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" customFormat="1">
@@ -945,7 +955,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5" customFormat="1">
@@ -1118,13 +1128,11 @@
       <c r="C23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1133,12 +1141,12 @@
         <v>11</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30">
       <c r="A25" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>4</v>
@@ -1149,90 +1157,167 @@
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="22" t="s">
+      <c r="B28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="23"/>
-      <c r="B27" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="23"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="23"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="23"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="23"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="23"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="5" t="s">
+      <c r="C32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="23"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="5" t="s">
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="23"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="5" t="s">
+      <c r="B34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="26"/>
-      <c r="B35" s="27"/>
+      <c r="B35" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C35" s="27"/>
-      <c r="D35" s="28" t="s">
-        <v>59</v>
-      </c>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="90">
+      <c r="A37" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="24"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="25"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="22"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="D40" s="28"/>
     </row>
   </sheetData>
   <sortState ref="A2:D20">

</xml_diff>

<commit_message>
agregué pequeños script para la visualizacion de los productos. actualice las tareas. REVISAR
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="65">
   <si>
     <t>TAREAS</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Buscador</t>
   </si>
   <si>
-    <t>Falta completar el funcionamiento del buscador.</t>
-  </si>
-  <si>
     <t>Listado de Productos con ordenamiento</t>
   </si>
   <si>
@@ -209,15 +206,16 @@
     <t>Validar entrada a la facturacion</t>
   </si>
   <si>
-    <t>Solo se prodra acceder a checkout01.php si primeramente en cart.php tiene artículos cargados.
-Solo se podrá acceder a checkout02.php si completó correctamente los datos de checkout01.php.
-Solo podrá acceder a factura.php y enviar correctamente el mail, si esta completo correctamente todo lo que existe en checkout02.php</t>
-  </si>
-  <si>
     <t>Agregar terminos y condiciones de una compra</t>
   </si>
   <si>
-    <t>Falta agregar el modal con el texto. Agregar estilos y el boton de cerrar.</t>
+    <t>Agregar que tiempo en la visualizacion de la compra</t>
+  </si>
+  <si>
+    <t>Agregar estilos a la factura</t>
+  </si>
+  <si>
+    <t>Falta modificarla para que mande la factura lo mas parecido a la web</t>
   </si>
 </sst>
 </file>
@@ -395,7 +393,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -452,16 +450,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -765,10 +766,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -810,7 +811,7 @@
     </row>
     <row r="3" spans="1:4" customFormat="1">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -819,7 +820,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" customFormat="1">
@@ -833,7 +834,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1">
@@ -873,17 +874,17 @@
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" customFormat="1">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>46</v>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" customFormat="1">
@@ -896,9 +897,7 @@
       <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" customFormat="1">
       <c r="A10" s="5" t="s">
@@ -911,7 +910,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" customFormat="1">
@@ -1004,7 +1003,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>34</v>
@@ -1035,7 +1034,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" customFormat="1">
@@ -1076,7 +1075,7 @@
     </row>
     <row r="23" spans="1:4" customFormat="1" ht="30">
       <c r="A23" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>4</v>
@@ -1088,7 +1087,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1097,12 +1096,12 @@
         <v>11</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30">
       <c r="A25" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>4</v>
@@ -1114,7 +1113,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>8</v>
@@ -1126,7 +1125,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>8</v>
@@ -1138,7 +1137,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>8</v>
@@ -1150,7 +1149,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>8</v>
@@ -1162,7 +1161,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>8</v>
@@ -1174,10 +1173,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>5</v>
@@ -1186,7 +1185,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>4</v>
@@ -1198,7 +1197,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>4</v>
@@ -1210,7 +1209,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>8</v>
@@ -1219,12 +1218,12 @@
         <v>11</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>4</v>
@@ -1233,45 +1232,61 @@
         <v>11</v>
       </c>
       <c r="D35" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="21" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="90">
-      <c r="A36" s="16" t="s">
+      <c r="B36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="B38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="9" t="s">
+      <c r="D39" s="24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="21"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="20"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="D39" s="23"/>
+    <row r="40" spans="1:4">
+      <c r="D40" s="20"/>
     </row>
   </sheetData>
   <sortState ref="A2:D20">

</xml_diff>

<commit_message>
actualizada las tareas + db actualizada
</commit_message>
<xml_diff>
--- a/_TAREAS.xlsx
+++ b/_TAREAS.xlsx
@@ -395,7 +395,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -462,9 +462,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -773,8 +770,8 @@
   </sheetPr>
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1232,18 +1229,18 @@
       <c r="A35" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="6" t="s">
+      <c r="B35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="90">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="24" t="s">
         <v>61</v>
       </c>
       <c r="B36" s="2" t="s">

</xml_diff>